<commit_message>
melhorada estilizacao da exportacao
</commit_message>
<xml_diff>
--- a/2022-10-21.xlsx
+++ b/2022-10-21.xlsx
@@ -28951,16 +28951,22 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD4B39"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -28973,7 +28979,7 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
       <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>

</xml_diff>